<commit_message>
feat: Add new scripts and update MMLU test results
- Add `fix_model_output_format.py` to correct formatting issues in model outputs.
- Add `test_fix_result.py` for testing the output correction script.
- Update `analyze_llm_results.py`, `generate_performance_excel.py`, and `visualize_performance.py` with new features and improvements.
- Update MMLU test results for all subjects based on the latest model outputs.
</commit_message>
<xml_diff>
--- a/subjects_perf_results/performance_summary.xlsx
+++ b/subjects_perf_results/performance_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>answer_not_found_count</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>avg_prompt_processing_rate_toks_per_sec</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>avg_token_generation_rate_toks_per_sec</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -470,6 +480,12 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>1084.062</v>
+      </c>
+      <c r="F2" t="n">
+        <v>34.395</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +502,12 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
+      <c r="E3" t="n">
+        <v>1002.025</v>
+      </c>
+      <c r="F3" t="n">
+        <v>35.127</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +524,12 @@
       <c r="D4" t="n">
         <v>2</v>
       </c>
+      <c r="E4" t="n">
+        <v>1081.163</v>
+      </c>
+      <c r="F4" t="n">
+        <v>34.709</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -518,6 +546,12 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
+      <c r="E5" t="n">
+        <v>1053.321</v>
+      </c>
+      <c r="F5" t="n">
+        <v>34.573</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +568,12 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="E6" t="n">
+        <v>986.223</v>
+      </c>
+      <c r="F6" t="n">
+        <v>34.907</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -550,6 +590,12 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>1068.248</v>
+      </c>
+      <c r="F7" t="n">
+        <v>35.063</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -566,6 +612,12 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>1143.015</v>
+      </c>
+      <c r="F8" t="n">
+        <v>34.641</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -582,6 +634,12 @@
       <c r="D9" t="n">
         <v>0</v>
       </c>
+      <c r="E9" t="n">
+        <v>1229.277</v>
+      </c>
+      <c r="F9" t="n">
+        <v>34.722</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -598,6 +656,12 @@
       <c r="D10" t="n">
         <v>3</v>
       </c>
+      <c r="E10" t="n">
+        <v>1087.439</v>
+      </c>
+      <c r="F10" t="n">
+        <v>30.123</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -614,6 +678,12 @@
       <c r="D11" t="n">
         <v>4</v>
       </c>
+      <c r="E11" t="n">
+        <v>1084.954</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30.877</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -630,6 +700,12 @@
       <c r="D12" t="n">
         <v>2</v>
       </c>
+      <c r="E12" t="n">
+        <v>1123.228</v>
+      </c>
+      <c r="F12" t="n">
+        <v>32.751</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -646,6 +722,12 @@
       <c r="D13" t="n">
         <v>0</v>
       </c>
+      <c r="E13" t="n">
+        <v>1106.721</v>
+      </c>
+      <c r="F13" t="n">
+        <v>35.083</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -662,6 +744,12 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
+      <c r="E14" t="n">
+        <v>971.568</v>
+      </c>
+      <c r="F14" t="n">
+        <v>34.295</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -678,6 +766,12 @@
       <c r="D15" t="n">
         <v>1</v>
       </c>
+      <c r="E15" t="n">
+        <v>1191.449</v>
+      </c>
+      <c r="F15" t="n">
+        <v>34.896</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -694,6 +788,12 @@
       <c r="D16" t="n">
         <v>0</v>
       </c>
+      <c r="E16" t="n">
+        <v>965.316</v>
+      </c>
+      <c r="F16" t="n">
+        <v>34.655</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -710,6 +810,12 @@
       <c r="D17" t="n">
         <v>4</v>
       </c>
+      <c r="E17" t="n">
+        <v>1054.102</v>
+      </c>
+      <c r="F17" t="n">
+        <v>30.669</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -726,6 +832,12 @@
       <c r="D18" t="n">
         <v>4</v>
       </c>
+      <c r="E18" t="n">
+        <v>1167.278</v>
+      </c>
+      <c r="F18" t="n">
+        <v>29.363</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -742,6 +854,12 @@
       <c r="D19" t="n">
         <v>1</v>
       </c>
+      <c r="E19" t="n">
+        <v>933.706</v>
+      </c>
+      <c r="F19" t="n">
+        <v>30.473</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -758,6 +876,12 @@
       <c r="D20" t="n">
         <v>1</v>
       </c>
+      <c r="E20" t="n">
+        <v>1066.96</v>
+      </c>
+      <c r="F20" t="n">
+        <v>30.997</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -774,6 +898,12 @@
       <c r="D21" t="n">
         <v>3</v>
       </c>
+      <c r="E21" t="n">
+        <v>1116.473</v>
+      </c>
+      <c r="F21" t="n">
+        <v>31.897</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -790,6 +920,12 @@
       <c r="D22" t="n">
         <v>0</v>
       </c>
+      <c r="E22" t="n">
+        <v>1171.724</v>
+      </c>
+      <c r="F22" t="n">
+        <v>30.879</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -806,6 +942,12 @@
       <c r="D23" t="n">
         <v>0</v>
       </c>
+      <c r="E23" t="n">
+        <v>1424.404</v>
+      </c>
+      <c r="F23" t="n">
+        <v>34.422</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -822,6 +964,12 @@
       <c r="D24" t="n">
         <v>1</v>
       </c>
+      <c r="E24" t="n">
+        <v>916.125</v>
+      </c>
+      <c r="F24" t="n">
+        <v>31.009</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -838,6 +986,12 @@
       <c r="D25" t="n">
         <v>0</v>
       </c>
+      <c r="E25" t="n">
+        <v>1082.054</v>
+      </c>
+      <c r="F25" t="n">
+        <v>34.603</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -854,6 +1008,12 @@
       <c r="D26" t="n">
         <v>6</v>
       </c>
+      <c r="E26" t="n">
+        <v>1026.389</v>
+      </c>
+      <c r="F26" t="n">
+        <v>31.054</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -870,6 +1030,12 @@
       <c r="D27" t="n">
         <v>13</v>
       </c>
+      <c r="E27" t="n">
+        <v>1023.598</v>
+      </c>
+      <c r="F27" t="n">
+        <v>26.652</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -886,6 +1052,12 @@
       <c r="D28" t="n">
         <v>3</v>
       </c>
+      <c r="E28" t="n">
+        <v>1015.448</v>
+      </c>
+      <c r="F28" t="n">
+        <v>30.234</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -902,6 +1074,12 @@
       <c r="D29" t="n">
         <v>9</v>
       </c>
+      <c r="E29" t="n">
+        <v>1156.026</v>
+      </c>
+      <c r="F29" t="n">
+        <v>29.792</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -918,6 +1096,12 @@
       <c r="D30" t="n">
         <v>2</v>
       </c>
+      <c r="E30" t="n">
+        <v>994.597</v>
+      </c>
+      <c r="F30" t="n">
+        <v>30.705</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -934,6 +1118,12 @@
       <c r="D31" t="n">
         <v>4</v>
       </c>
+      <c r="E31" t="n">
+        <v>1249.841</v>
+      </c>
+      <c r="F31" t="n">
+        <v>32.179</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -950,6 +1140,12 @@
       <c r="D32" t="n">
         <v>0</v>
       </c>
+      <c r="E32" t="n">
+        <v>1381.203</v>
+      </c>
+      <c r="F32" t="n">
+        <v>29.941</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -966,6 +1162,12 @@
       <c r="D33" t="n">
         <v>1</v>
       </c>
+      <c r="E33" t="n">
+        <v>1398.54</v>
+      </c>
+      <c r="F33" t="n">
+        <v>32.461</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -982,6 +1184,12 @@
       <c r="D34" t="n">
         <v>1</v>
       </c>
+      <c r="E34" t="n">
+        <v>910.004</v>
+      </c>
+      <c r="F34" t="n">
+        <v>30.385</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -998,6 +1206,12 @@
       <c r="D35" t="n">
         <v>2</v>
       </c>
+      <c r="E35" t="n">
+        <v>977.5309999999999</v>
+      </c>
+      <c r="F35" t="n">
+        <v>34.06</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1014,6 +1228,12 @@
       <c r="D36" t="n">
         <v>0</v>
       </c>
+      <c r="E36" t="n">
+        <v>1117.798</v>
+      </c>
+      <c r="F36" t="n">
+        <v>33.402</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1030,6 +1250,12 @@
       <c r="D37" t="n">
         <v>0</v>
       </c>
+      <c r="E37" t="n">
+        <v>1046.693</v>
+      </c>
+      <c r="F37" t="n">
+        <v>33.347</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1046,6 +1272,12 @@
       <c r="D38" t="n">
         <v>0</v>
       </c>
+      <c r="E38" t="n">
+        <v>1041.886</v>
+      </c>
+      <c r="F38" t="n">
+        <v>34.191</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1062,6 +1294,12 @@
       <c r="D39" t="n">
         <v>1</v>
       </c>
+      <c r="E39" t="n">
+        <v>1090.118</v>
+      </c>
+      <c r="F39" t="n">
+        <v>33.842</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1078,6 +1316,12 @@
       <c r="D40" t="n">
         <v>0</v>
       </c>
+      <c r="E40" t="n">
+        <v>1103.062</v>
+      </c>
+      <c r="F40" t="n">
+        <v>34.297</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1094,6 +1338,12 @@
       <c r="D41" t="n">
         <v>0</v>
       </c>
+      <c r="E41" t="n">
+        <v>988.217</v>
+      </c>
+      <c r="F41" t="n">
+        <v>34.135</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1110,6 +1360,12 @@
       <c r="D42" t="n">
         <v>0</v>
       </c>
+      <c r="E42" t="n">
+        <v>979.915</v>
+      </c>
+      <c r="F42" t="n">
+        <v>34.334</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1126,6 +1382,12 @@
       <c r="D43" t="n">
         <v>6</v>
       </c>
+      <c r="E43" t="n">
+        <v>1020.68</v>
+      </c>
+      <c r="F43" t="n">
+        <v>31.375</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1142,6 +1404,12 @@
       <c r="D44" t="n">
         <v>5</v>
       </c>
+      <c r="E44" t="n">
+        <v>1018.988</v>
+      </c>
+      <c r="F44" t="n">
+        <v>31.759</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1158,6 +1426,12 @@
       <c r="D45" t="n">
         <v>57</v>
       </c>
+      <c r="E45" t="n">
+        <v>1332.386</v>
+      </c>
+      <c r="F45" t="n">
+        <v>27.28</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1174,6 +1448,12 @@
       <c r="D46" t="n">
         <v>1</v>
       </c>
+      <c r="E46" t="n">
+        <v>1012.249</v>
+      </c>
+      <c r="F46" t="n">
+        <v>30.572</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1190,6 +1470,12 @@
       <c r="D47" t="n">
         <v>1</v>
       </c>
+      <c r="E47" t="n">
+        <v>941.836</v>
+      </c>
+      <c r="F47" t="n">
+        <v>30.668</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1206,6 +1492,12 @@
       <c r="D48" t="n">
         <v>2</v>
       </c>
+      <c r="E48" t="n">
+        <v>1026.975</v>
+      </c>
+      <c r="F48" t="n">
+        <v>33.756</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1222,6 +1514,12 @@
       <c r="D49" t="n">
         <v>7</v>
       </c>
+      <c r="E49" t="n">
+        <v>1170.773</v>
+      </c>
+      <c r="F49" t="n">
+        <v>29.284</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1238,6 +1536,12 @@
       <c r="D50" t="n">
         <v>5</v>
       </c>
+      <c r="E50" t="n">
+        <v>1322.373</v>
+      </c>
+      <c r="F50" t="n">
+        <v>30.118</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1254,6 +1558,12 @@
       <c r="D51" t="n">
         <v>2</v>
       </c>
+      <c r="E51" t="n">
+        <v>1305.003</v>
+      </c>
+      <c r="F51" t="n">
+        <v>31.761</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1270,6 +1580,12 @@
       <c r="D52" t="n">
         <v>4</v>
       </c>
+      <c r="E52" t="n">
+        <v>1044.689</v>
+      </c>
+      <c r="F52" t="n">
+        <v>30.545</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1286,6 +1602,12 @@
       <c r="D53" t="n">
         <v>0</v>
       </c>
+      <c r="E53" t="n">
+        <v>1030.866</v>
+      </c>
+      <c r="F53" t="n">
+        <v>33.282</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1302,6 +1624,12 @@
       <c r="D54" t="n">
         <v>1</v>
       </c>
+      <c r="E54" t="n">
+        <v>1256.453</v>
+      </c>
+      <c r="F54" t="n">
+        <v>33.187</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1318,6 +1646,12 @@
       <c r="D55" t="n">
         <v>0</v>
       </c>
+      <c r="E55" t="n">
+        <v>1004.054</v>
+      </c>
+      <c r="F55" t="n">
+        <v>30.713</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1334,6 +1668,12 @@
       <c r="D56" t="n">
         <v>0</v>
       </c>
+      <c r="E56" t="n">
+        <v>969.98</v>
+      </c>
+      <c r="F56" t="n">
+        <v>34.442</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1350,6 +1690,12 @@
       <c r="D57" t="n">
         <v>0</v>
       </c>
+      <c r="E57" t="n">
+        <v>975.877</v>
+      </c>
+      <c r="F57" t="n">
+        <v>33.597</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1365,6 +1711,34 @@
       </c>
       <c r="D58" t="n">
         <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>936.898</v>
+      </c>
+      <c r="F58" t="n">
+        <v>33.577</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>14042</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.5151021008403361</v>
+      </c>
+      <c r="D59" t="n">
+        <v>160</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1113.612968380573</v>
+      </c>
+      <c r="F59" t="n">
+        <v>31.50770801880074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>